<commit_message>
Make Solving async and work on last layer solving
</commit_message>
<xml_diff>
--- a/docs/PllPatternGenerator.xlsx
+++ b/docs/PllPatternGenerator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\Rubinator3000\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13782D90-FBE5-497B-8AD0-E4BB9C5C8293}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58222C98-3281-4180-A77A-475E265ABC3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13290" xr2:uid="{2FFD1324-8666-461E-9AD9-46C91CBD5110}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{2FFD1324-8666-461E-9AD9-46C91CBD5110}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -454,12 +454,13 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="10" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -485,7 +486,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="G2" t="s">
         <v>16</v>
       </c>
@@ -499,7 +500,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -507,14 +508,14 @@
         <v>3</v>
       </c>
       <c r="D3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="G3">
         <f>MOD(C3-D3+4, 4)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H3">
         <f>MOD(C3-E3+4,4)</f>
@@ -522,14 +523,14 @@
       </c>
       <c r="I3">
         <f>MOD(D3-E3+4,4)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K3">
         <f>G3+H3*4+I3*16</f>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -537,14 +538,14 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="G4">
         <f t="shared" ref="G4:G6" si="0">MOD(C4-D4+4, 4)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H4">
         <f t="shared" ref="H4:H6" si="1">MOD(C4-E4+4,4)</f>
@@ -552,14 +553,14 @@
       </c>
       <c r="I4">
         <f t="shared" ref="I4:I6" si="2">MOD(D4-E4+4,4)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K4">
         <f t="shared" ref="K4:K6" si="3">G4+H4*4+I4*16</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -567,14 +568,14 @@
         <v>2</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E5">
         <v>3</v>
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H5">
         <f t="shared" si="1"/>
@@ -582,14 +583,14 @@
       </c>
       <c r="I5">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K5">
         <f t="shared" si="3"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -597,14 +598,14 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E6">
         <v>2</v>
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H6">
         <f t="shared" si="1"/>
@@ -612,14 +613,14 @@
       </c>
       <c r="I6">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K6">
         <f t="shared" si="3"/>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -627,7 +628,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -635,7 +636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -643,7 +644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -651,7 +652,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Fix .csproj and optimize face rotation
</commit_message>
<xml_diff>
--- a/docs/PllPatternGenerator.xlsx
+++ b/docs/PllPatternGenerator.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\Rubinator3000\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Philipp\Source\Repos\Rubinator3000\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58222C98-3281-4180-A77A-475E265ABC3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC96946-F4D4-4854-A651-9B8D5035F42D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{2FFD1324-8666-461E-9AD9-46C91CBD5110}"/>
   </bookViews>
@@ -451,13 +451,13 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="10" width="0" hidden="1" customWidth="1"/>
+    <col min="6" max="10" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -505,29 +505,29 @@
         <v>5</v>
       </c>
       <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
         <v>3</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="G3">
         <f>MOD(C3-D3+4, 4)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H3">
         <f>MOD(C3-E3+4,4)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I3">
         <f>MOD(D3-E3+4,4)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K3">
         <f>G3+H3*4+I3*16</f>
-        <v>30</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -538,14 +538,14 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="G4">
         <f t="shared" ref="G4:G6" si="0">MOD(C4-D4+4, 4)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H4">
         <f t="shared" ref="H4:H6" si="1">MOD(C4-E4+4,4)</f>
@@ -553,11 +553,11 @@
       </c>
       <c r="I4">
         <f t="shared" ref="I4:I6" si="2">MOD(D4-E4+4,4)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K4">
         <f t="shared" ref="K4:K6" si="3">G4+H4*4+I4*16</f>
-        <v>34</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -568,26 +568,26 @@
         <v>2</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H5">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I5">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5">
         <f t="shared" si="3"/>
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -595,13 +595,13 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
@@ -609,15 +609,15 @@
       </c>
       <c r="H6">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K6">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">

</xml_diff>